<commit_message>
Clarify comments.  On branch amarchan_ares_schematic_review  Your branch is ahead of 'origin/amarchan_ares_schematic_review' by 1 commit.    (use "git push" to publish your local commits)
 Changes to be committed:
	modified:   ../doc/schematic_review/ares_xc7a50t_1582747176.xlsx
</commit_message>
<xml_diff>
--- a/doc/schematic_review/ares_xc7a50t_1582747176.xlsx
+++ b/doc/schematic_review/ares_xc7a50t_1582747176.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="646">
   <si>
     <t>#Top: ares_pcie   Floorplan: impl_1   Part: xc7a50ticpg236-1L</t>
   </si>
@@ -1901,28 +1901,58 @@
     <t>G7</t>
   </si>
   <si>
-    <t>Not Connected</t>
-  </si>
-  <si>
     <t>Check the tree. Why connected to EHL?</t>
   </si>
   <si>
-    <t>Check if any chip support WP_N</t>
-  </si>
-  <si>
-    <t>Check if any chip support this</t>
-  </si>
-  <si>
-    <t>Rename?</t>
-  </si>
-  <si>
-    <t>Rename. Pull-up?</t>
-  </si>
-  <si>
-    <t>Not connected</t>
-  </si>
-  <si>
     <t>PWRST, Should be connected to H1 bank 35</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Check if any chip support this functionality</t>
+  </si>
+  <si>
+    <t>Rename to a more generic name? EHL_GPIO_0?</t>
+  </si>
+  <si>
+    <t>Do we need a pullup Rename to a more generic name? EHL_GPIO_0?</t>
+  </si>
+  <si>
+    <t>Disconnect the PLTRSTN and connect to bank 35 Pin J1</t>
+  </si>
+  <si>
+    <t>Not Connected. See note above on pin L17</t>
+  </si>
+  <si>
+    <t>Not connected. See note above on pin B17</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[2]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[4]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[3]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[0]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[7]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[5]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to hb_dq[1]</t>
+  </si>
+  <si>
+    <t>[amarchan]: Change vivado constrain to  hb_dq[6]</t>
+  </si>
+  <si>
+    <t>Clarify what we do with that signal</t>
   </si>
 </sst>
 </file>
@@ -8056,15 +8086,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A211" activeCellId="4" sqref="A181:XFD181 A190:XFD190 A197:XFD197 A203:XFD203 A211:XFD211"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
@@ -8095,6 +8125,9 @@
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>630</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9222,7 +9255,7 @@
         <v>92</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>87</v>
+        <v>637</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>95</v>
@@ -9263,7 +9296,7 @@
         <v>88</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>79</v>
+        <v>638</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>91</v>
@@ -9304,7 +9337,7 @@
         <v>84</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>83</v>
+        <v>639</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>87</v>
@@ -9345,7 +9378,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>95</v>
+        <v>640</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>83</v>
@@ -9386,7 +9419,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>66</v>
+        <v>641</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>79</v>
@@ -9427,7 +9460,7 @@
         <v>72</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>75</v>
+        <v>642</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>75</v>
@@ -9468,7 +9501,7 @@
         <v>68</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>91</v>
+        <v>643</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>71</v>
@@ -9509,7 +9542,7 @@
         <v>62</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>71</v>
+        <v>644</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>66</v>
@@ -9681,7 +9714,7 @@
         <v>320</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>323</v>
@@ -9719,7 +9752,7 @@
         <v>300</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>303</v>
@@ -10125,6 +10158,9 @@
       <c r="B71" s="3" t="s">
         <v>401</v>
       </c>
+      <c r="C71" s="3" t="s">
+        <v>634</v>
+      </c>
       <c r="E71" s="3" t="s">
         <v>403</v>
       </c>
@@ -10514,6 +10550,9 @@
       <c r="B90" s="3" t="s">
         <v>292</v>
       </c>
+      <c r="C90" s="3" t="s">
+        <v>645</v>
+      </c>
       <c r="D90" s="3" t="s">
         <v>295</v>
       </c>
@@ -10540,6 +10579,9 @@
       <c r="B91" s="3" t="s">
         <v>268</v>
       </c>
+      <c r="C91" s="3" t="s">
+        <v>645</v>
+      </c>
       <c r="D91" s="3" t="s">
         <v>271</v>
       </c>
@@ -10584,7 +10626,7 @@
         <v>441</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>443</v>
@@ -11635,7 +11677,7 @@
         <v>179</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>183</v>
@@ -11667,7 +11709,7 @@
         <v>153</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
Excel spreadsheet was not saved in previous commit
</commit_message>
<xml_diff>
--- a/doc/schematic_review/ares_xc7a50t_1582747176.xlsx
+++ b/doc/schematic_review/ares_xc7a50t_1582747176.xlsx
@@ -8086,7 +8086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
@@ -8094,7 +8094,7 @@
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>

</xml_diff>